<commit_message>
Modificación modelo, nuevas células
</commit_message>
<xml_diff>
--- a/public/assets/modelo-nomina.xlsx
+++ b/public/assets/modelo-nomina.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fedek\OneDrive\Escritorio\Programación\mac-aegis\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53921CC3-9AEB-4510-AAF5-A83F5A638C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358497F-F89D-49B7-8600-F447259F671C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="base" sheetId="1" r:id="rId1"/>
     <sheet name="listas" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Proceso">listas!$B$2:$B$5</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Exa</t>
   </si>
@@ -83,13 +86,22 @@
   </si>
   <si>
     <t>Cecor</t>
+  </si>
+  <si>
+    <t>CD Uy</t>
+  </si>
+  <si>
+    <t>Célula 608</t>
+  </si>
+  <si>
+    <t>Célula 687</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +113,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -441,7 +459,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,10 +488,10 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,21 +963,21 @@
       <c r="D80" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D80" xr:uid="{D2AB18DA-9161-4D69-BD8A-A451E8A03A55}">
+      <formula1>Proceso</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E3DDE6F6-D3AF-4EA5-A8DF-6F542A9CEC1F}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A29CE9C2-441C-4D8A-809D-E5F17F4823BB}">
           <x14:formula1>
-            <xm:f>listas!$A$2:$A$13</xm:f>
+            <xm:f>listas!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C80</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C7C98B54-57FC-42D1-B98F-4DAB36EB83FF}">
-          <x14:formula1>
-            <xm:f>listas!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D80</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -969,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EE8B76-7B24-4265-AAEB-47DC595027AC}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,6 +1035,9 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1056,6 +1077,16 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifica la carga de asesor
</commit_message>
<xml_diff>
--- a/public/assets/modelo-nomina.xlsx
+++ b/public/assets/modelo-nomina.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fedek\OneDrive\Escritorio\Programación\mac-aegis\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fedek\OneDrive\Escritorio\Programación\Mac Aegis\Front\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358497F-F89D-49B7-8600-F447259F671C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839F1F7F-29B6-4C2F-96CA-AD904F501D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="listas" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Proceso">listas!$B$2:$B$5</definedName>
+    <definedName name="Proceso">listas!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Exa</t>
   </si>
@@ -40,28 +40,10 @@
     <t>Célula</t>
   </si>
   <si>
-    <t>Proceso</t>
-  </si>
-  <si>
-    <t>Célula 604</t>
-  </si>
-  <si>
-    <t>Célula 611</t>
-  </si>
-  <si>
-    <t>Célula 679</t>
-  </si>
-  <si>
-    <t>Célula 677</t>
-  </si>
-  <si>
     <t>Célula 630</t>
   </si>
   <si>
     <t>Célula 662</t>
-  </si>
-  <si>
-    <t>Célula 668</t>
   </si>
   <si>
     <t>Célula 669</t>
@@ -77,24 +59,6 @@
   </si>
   <si>
     <t>Célula 685</t>
-  </si>
-  <si>
-    <t>CD Ar</t>
-  </si>
-  <si>
-    <t>Cecor UY</t>
-  </si>
-  <si>
-    <t>Cecor</t>
-  </si>
-  <si>
-    <t>CD Uy</t>
-  </si>
-  <si>
-    <t>Célula 608</t>
-  </si>
-  <si>
-    <t>Célula 687</t>
   </si>
 </sst>
 </file>
@@ -456,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +431,9 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -480,502 +443,413 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D80" xr:uid="{D2AB18DA-9161-4D69-BD8A-A451E8A03A55}">
-      <formula1>Proceso</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A29CE9C2-441C-4D8A-809D-E5F17F4823BB}">
           <x14:formula1>
-            <xm:f>listas!$A$2:$A$15</xm:f>
+            <xm:f>listas!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C80</xm:sqref>
         </x14:dataValidation>
@@ -987,106 +861,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EE8B76-7B24-4265-AAEB-47DC595027AC}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>